<commit_message>
Tested Agency Completion Added new excel sheet for completion functionality
</commit_message>
<xml_diff>
--- a/updated.xlsx
+++ b/updated.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" state="visible" r:id="rId1"/>
@@ -8661,8 +8661,8 @@
   </sheetPr>
   <dimension ref="A1:H427"/>
   <sheetViews>
-    <sheetView topLeftCell="A426" workbookViewId="0">
-      <selection activeCell="C426" sqref="C426"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
@@ -18513,7 +18513,7 @@
   </sheetPr>
   <dimension ref="A1:H426"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
@@ -58293,8 +58293,8 @@
   </sheetPr>
   <dimension ref="A1:H426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>

</xml_diff>